<commit_message>
Stock_Fund Ver 0.1.5 : Modify stock app style and text size
</commit_message>
<xml_diff>
--- a/174444_指標選擇0614.xlsx
+++ b/174444_指標選擇0614.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ntutedutw-my.sharepoint.com/personal/t106ab0031_ntut_edu_tw/Documents/Self-Learning/ETF智能選股/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\NTUT\Case\CMoney\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="8_{3AF831F2-CDE2-403A-8AAD-F0F2D93A59A1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{0D2F307A-2E1F-4489-ACCE-C5E60817C059}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9578E622-E2F2-4FA9-AD76-A6B7CB011C28}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{CC67D7B3-D66C-4A84-8E9C-CC3D7C43E05F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CC67D7B3-D66C-4A84-8E9C-CC3D7C43E05F}"/>
   </bookViews>
   <sheets>
     <sheet name="基金" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>指標一</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -60,23 +60,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>指標四</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>一年</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>二年</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>三年</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>五年</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -262,13 +250,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -586,231 +574,217 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6704B21A-AC0A-4670-95D5-0F208120CCAA}">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:H14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G3" t="s">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
       </c>
       <c r="H5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>34</v>
       </c>
-      <c r="B13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
         <v>35</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -830,72 +804,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B9F1C44-4D45-474D-B4FB-B3BE96CFCF1B}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stock_Fund Ver 0.1.7 : fund api test
</commit_message>
<xml_diff>
--- a/174444_指標選擇0614.xlsx
+++ b/174444_指標選擇0614.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\NTUT\Case\CMoney\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMoney\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9578E622-E2F2-4FA9-AD76-A6B7CB011C28}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F382DE1-9CEC-4F3D-87CD-DEAFAE72BA63}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CC67D7B3-D66C-4A84-8E9C-CC3D7C43E05F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CC67D7B3-D66C-4A84-8E9C-CC3D7C43E05F}"/>
   </bookViews>
   <sheets>
     <sheet name="基金" sheetId="1" r:id="rId1"/>
@@ -575,17 +575,17 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:D8"/>
+      <selection activeCell="D8" sqref="C2:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -605,7 +605,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>29</v>
       </c>
@@ -623,7 +623,7 @@
       </c>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -649,7 +649,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -675,7 +675,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -701,7 +701,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -727,7 +727,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>4</v>
       </c>
@@ -741,7 +741,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>17</v>
       </c>
@@ -755,7 +755,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E9" t="s">
         <v>23</v>
       </c>
@@ -763,7 +763,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -771,7 +771,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -779,7 +779,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -808,12 +808,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>36</v>
       </c>
@@ -824,7 +824,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -832,7 +832,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -840,7 +840,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -848,7 +848,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -856,7 +856,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -864,7 +864,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>

</xml_diff>